<commit_message>
Gean - Email - PDF - Excel
</commit_message>
<xml_diff>
--- a/build/web/resources/Office/excel/produtos.xlsx
+++ b/build/web/resources/Office/excel/produtos.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="13">
   <si>
     <t>Code</t>
   </si>
@@ -70,7 +70,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -79,6 +79,11 @@
     </fill>
     <fill>
       <patternFill>
+        <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="22"/>
       </patternFill>
     </fill>
@@ -105,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="center" vertical="center"/>
@@ -117,6 +122,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
@@ -428,123 +442,123 @@
   <sheetFormatPr defaultRowHeight="20.0" baseColWidth="15" customHeight="true"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="n">
+      <c r="A2" s="8" t="n">
         <v>1.0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="n">
+      <c r="C2" s="9" t="n">
         <v>200.5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="n">
+      <c r="A3" s="8" t="n">
         <v>2.0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6" t="n">
+      <c r="C3" s="9" t="n">
         <v>1050.5</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="n">
+      <c r="A4" s="8" t="n">
         <v>3.0</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6" t="n">
+      <c r="C4" s="9" t="n">
         <v>50.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="n">
+      <c r="A5" s="8" t="n">
         <v>4.0</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6" t="n">
+      <c r="C5" s="9" t="n">
         <v>200.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="n">
+      <c r="A6" s="8" t="n">
         <v>5.0</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6" t="n">
+      <c r="C6" s="9" t="n">
         <v>450.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="n">
+      <c r="A7" s="8" t="n">
         <v>6.0</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6" t="n">
+      <c r="C7" s="9" t="n">
         <v>150.5</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="n">
+      <c r="A8" s="8" t="n">
         <v>7.0</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="6" t="n">
+      <c r="C8" s="9" t="n">
         <v>300.99</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="8" t="n">
         <v>8.0</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="6" t="n">
+      <c r="C9" s="9" t="n">
         <v>1000.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="n">
+      <c r="A10" s="8" t="n">
         <v>9.0</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="6" t="n">
+      <c r="C10" s="9" t="n">
         <v>350.0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="n">
+      <c r="A11" s="8" t="n">
         <v>10.0</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="6" t="n">
+      <c r="C11" s="9" t="n">
         <v>200.0</v>
       </c>
     </row>

</xml_diff>